<commit_message>
fix test-suite miss product & update test-job columns display
</commit_message>
<xml_diff>
--- a/public/template2.xlsx
+++ b/public/template2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangdongming/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3882ABD5-8246-FD4B-95B8-2AE25D53E3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9ADF8-DC78-2A4C-8C97-BEB55C9BA2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44320" yWindow="5480" windowWidth="28240" windowHeight="17440" xr2:uid="{A974E53D-0082-094F-8882-32A1A1B741D5}"/>
+    <workbookView xWindow="-38080" yWindow="2920" windowWidth="28240" windowHeight="17440" xr2:uid="{AD59BCEE-0A2B-7340-A783-F9FD3A098522}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>用户说</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>技能</t>
@@ -48,11 +49,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>joss平台分享url（非必需）</t>
+    <t>测试用例优先级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>测试用例优先级</t>
+    <t>joss平台分享url</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -416,45 +417,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17701650-7C5A-B94A-A00D-6F4E8C88DCA6}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E2E3D0-4468-9048-BEC8-129F04AFC06D}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{1CE9227A-FF81-1F41-A71E-DAB03EAD273A}">
+      <formula1>"1,2,3,4"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>